<commit_message>
SUMIF for titanic passenger classes
</commit_message>
<xml_diff>
--- a/Basic Analysis/Conditional Aggregations/Conditional aggregation -Countif Sumif.xlsx
+++ b/Basic Analysis/Conditional Aggregations/Conditional aggregation -Countif Sumif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Friedturnip\Desktop\Data Foundations BUILD\Aggregating Data\Conditional formulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Basic Analysis\Conditional Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBCBE39B-3374-45E2-825B-3E4A89E686A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46048DC-C277-4D0D-A26A-AF54B6241AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="27675" windowHeight="14760" xr2:uid="{BABEADB7-7078-4DBD-96F0-BD090558A0C5}"/>
+    <workbookView xWindow="2340" yWindow="420" windowWidth="29850" windowHeight="14805" xr2:uid="{BABEADB7-7078-4DBD-96F0-BD090558A0C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Titanic Passengers" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3571" uniqueCount="912">
   <si>
     <t>Survived</t>
   </si>
@@ -2767,6 +2758,9 @@
   </si>
   <si>
     <t>AVG</t>
+  </si>
+  <si>
+    <t>Total Passangers</t>
   </si>
 </sst>
 </file>
@@ -2858,7 +2852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2884,6 +2878,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2894,15 +2892,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3310,7 +3305,7 @@
   <dimension ref="A1:V888"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,6 +3317,7 @@
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -3605,24 +3601,27 @@
       <c r="F14" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="16" t="s">
         <v>900</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="5" t="s">
         <v>901</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="R14" s="12" t="s">
+      <c r="O14" s="17" t="s">
+        <v>911</v>
+      </c>
+      <c r="R14" s="14" t="s">
         <v>900</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
       <c r="V14" s="7" t="s">
         <v>901</v>
       </c>
@@ -3646,21 +3645,33 @@
       <c r="F15" s="4">
         <v>31.274999999999999</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="13" t="s">
         <v>903</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="17"/>
-      <c r="R15" s="11" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="6">
+        <f>COUNTIF(A2:A888,"Yes")</f>
+        <v>342</v>
+      </c>
+      <c r="N15" s="12">
+        <f>M15/887</f>
+        <v>0.38556933483652761</v>
+      </c>
+      <c r="O15">
+        <v>887</v>
+      </c>
+      <c r="R15" s="13" t="s">
         <v>905</v>
       </c>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="6"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="18">
+        <f>SUMIF(B:B,"First",F:F)</f>
+        <v>18177.412499999984</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3681,21 +3692,30 @@
       <c r="F16" s="4">
         <v>7.8541999999999996</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="13" t="s">
         <v>904</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="17"/>
-      <c r="R16" s="11" t="s">
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="6">
+        <f>COUNTIF(B2:B888,"First")</f>
+        <v>216</v>
+      </c>
+      <c r="N16" s="12">
+        <f>M16/887</f>
+        <v>0.24351747463359638</v>
+      </c>
+      <c r="R16" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="6"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="18">
+        <f>SUMIF(B:B,"Second",F:F)</f>
+        <v>3801.8416999999995</v>
+      </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -3716,13 +3736,16 @@
       <c r="F17" s="4">
         <v>16</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="R17" s="13" t="s">
         <v>907</v>
       </c>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="6"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="18">
+        <f>SUMIF(B:B,"Third",F:F)</f>
+        <v>6675.6535000000022</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -3931,7 +3954,7 @@
       <c r="F26" s="4">
         <v>21.074999999999999</v>
       </c>
-      <c r="O26" s="16"/>
+      <c r="O26" s="11"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">

</xml_diff>

<commit_message>
Add worksheet on multiple CountIFs
</commit_message>
<xml_diff>
--- a/Basic Analysis/Conditional Aggregations/Conditional aggregation -Countif Sumif.xlsx
+++ b/Basic Analysis/Conditional Aggregations/Conditional aggregation -Countif Sumif.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Basic Analysis\Conditional Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46048DC-C277-4D0D-A26A-AF54B6241AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8833167-29E4-40BC-A77B-E11E6F1E8493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="420" windowWidth="29850" windowHeight="14805" xr2:uid="{BABEADB7-7078-4DBD-96F0-BD090558A0C5}"/>
   </bookViews>
@@ -2882,6 +2882,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2892,8 +2894,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:V888"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,27 +3601,27 @@
       <c r="F14" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="18" t="s">
         <v>900</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="5" t="s">
         <v>901</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="13" t="s">
         <v>911</v>
       </c>
-      <c r="R14" s="14" t="s">
+      <c r="R14" s="16" t="s">
         <v>900</v>
       </c>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
       <c r="V14" s="7" t="s">
         <v>901</v>
       </c>
@@ -3645,12 +3645,12 @@
       <c r="F15" s="4">
         <v>31.274999999999999</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="15" t="s">
         <v>903</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
       <c r="M15" s="6">
         <f>COUNTIF(A2:A888,"Yes")</f>
         <v>342</v>
@@ -3662,13 +3662,13 @@
       <c r="O15">
         <v>887</v>
       </c>
-      <c r="R15" s="13" t="s">
+      <c r="R15" s="15" t="s">
         <v>905</v>
       </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="18">
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="14">
         <f>SUMIF(B:B,"First",F:F)</f>
         <v>18177.412499999984</v>
       </c>
@@ -3692,12 +3692,12 @@
       <c r="F16" s="4">
         <v>7.8541999999999996</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="15" t="s">
         <v>904</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
       <c r="M16" s="6">
         <f>COUNTIF(B2:B888,"First")</f>
         <v>216</v>
@@ -3706,13 +3706,13 @@
         <f>M16/887</f>
         <v>0.24351747463359638</v>
       </c>
-      <c r="R16" s="13" t="s">
+      <c r="R16" s="15" t="s">
         <v>906</v>
       </c>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="18">
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="14">
         <f>SUMIF(B:B,"Second",F:F)</f>
         <v>3801.8416999999995</v>
       </c>
@@ -3736,13 +3736,13 @@
       <c r="F17" s="4">
         <v>16</v>
       </c>
-      <c r="R17" s="13" t="s">
+      <c r="R17" s="15" t="s">
         <v>907</v>
       </c>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="18">
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="14">
         <f>SUMIF(B:B,"Third",F:F)</f>
         <v>6675.6535000000022</v>
       </c>
@@ -3839,9 +3839,18 @@
       <c r="R21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
+      <c r="S21" s="6">
+        <f>SUMIF(B:B,R21,F:F)</f>
+        <v>18177.412499999984</v>
+      </c>
+      <c r="T21" s="6">
+        <f>COUNTIF(B:B,R21)</f>
+        <v>216</v>
+      </c>
+      <c r="U21" s="14">
+        <f>S21/T21</f>
+        <v>84.154687499999923</v>
+      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -3865,9 +3874,18 @@
       <c r="R22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
+      <c r="S22" s="6">
+        <f t="shared" ref="S22:S23" si="0">SUMIF(B:B,R22,F:F)</f>
+        <v>3801.8416999999995</v>
+      </c>
+      <c r="T22" s="6">
+        <f t="shared" ref="T22:T23" si="1">COUNTIF(B:B,R22)</f>
+        <v>184</v>
+      </c>
+      <c r="U22" s="14">
+        <f t="shared" ref="U22:U23" si="2">S22/T22</f>
+        <v>20.66218315217391</v>
+      </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -3891,9 +3909,18 @@
       <c r="R23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
+      <c r="S23" s="6">
+        <f t="shared" si="0"/>
+        <v>6675.6535000000022</v>
+      </c>
+      <c r="T23" s="6">
+        <f t="shared" si="1"/>
+        <v>487</v>
+      </c>
+      <c r="U23" s="14">
+        <f t="shared" si="2"/>
+        <v>13.707707392197129</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">

</xml_diff>